<commit_message>
merged changes and completed ORA with extra figs, added IPA analysis
</commit_message>
<xml_diff>
--- a/3_output/GO_sig.xlsx
+++ b/3_output/GO_sig.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="DT vs PBS" sheetId="1" r:id="rId1"/>
-    <sheet name="Treg vs PBS" sheetId="2" r:id="rId2"/>
-    <sheet name="Treg vs DT" sheetId="3" r:id="rId3"/>
+    <sheet name="DT vs veh" sheetId="1" r:id="rId1"/>
+    <sheet name="DT+Treg vs veh" sheetId="2" r:id="rId2"/>
+    <sheet name="DT+Treg vs DT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
Large update with final visualisations
</commit_message>
<xml_diff>
--- a/3_output/GO_sig.xlsx
+++ b/3_output/GO_sig.xlsx
@@ -471,13 +471,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>4.271109068344356e-12</v>
+        <v>4.271109068344356E-12</v>
       </c>
       <c r="H2">
-        <v>1.727663618145292e-08</v>
+        <v>1.727663618145292E-08</v>
       </c>
       <c r="I2">
-        <v>1.504329572913707e-08</v>
+        <v>1.504329572913707E-08</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -535,13 +535,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>8.585460182855733e-12</v>
+        <v>8.585460182855733E-12</v>
       </c>
       <c r="H3">
-        <v>1.736409321982572e-08</v>
+        <v>1.736409321982572E-08</v>
       </c>
       <c r="I3">
-        <v>1.511944724833436e-08</v>
+        <v>1.511944724833436E-08</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -600,13 +600,13 @@
         </is>
       </c>
       <c r="G4">
-        <v>4.164689447143572e-11</v>
+        <v>4.164689447143572E-11</v>
       </c>
       <c r="H4">
-        <v>5.615389604565249e-08</v>
+        <v>5.615389604565249E-08</v>
       </c>
       <c r="I4">
-        <v>4.889491540400839e-08</v>
+        <v>4.889491540400839E-08</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -650,13 +650,13 @@
         </is>
       </c>
       <c r="G5">
-        <v>6.621751738380069e-11</v>
+        <v>6.621751738380069E-11</v>
       </c>
       <c r="H5">
-        <v>6.688153714324598e-08</v>
+        <v>6.688153714324598E-08</v>
       </c>
       <c r="I5">
-        <v>5.823580073679034e-08</v>
+        <v>5.823580073679034E-08</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -714,13 +714,13 @@
         </is>
       </c>
       <c r="G6">
-        <v>8.26718629706378e-11</v>
+        <v>8.26718629706378E-11</v>
       </c>
       <c r="H6">
-        <v>6.688153714324598e-08</v>
+        <v>6.688153714324598E-08</v>
       </c>
       <c r="I6">
-        <v>5.823580073679034e-08</v>
+        <v>5.823580073679034E-08</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -778,13 +778,13 @@
         </is>
       </c>
       <c r="G7">
-        <v>3.136301604559533e-09</v>
+        <v>3.136301604559533E-09</v>
       </c>
       <c r="H7">
-        <v>2.114389998407219e-06</v>
+        <v>2.114389998407219E-06</v>
       </c>
       <c r="I7">
-        <v>1.841064064711614e-06</v>
+        <v>1.841064064711614E-06</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -842,13 +842,13 @@
         </is>
       </c>
       <c r="G8">
-        <v>7.2343428486282e-09</v>
+        <v>7.2343428486282E-09</v>
       </c>
       <c r="H8">
-        <v>4.180416688957296e-06</v>
+        <v>4.180416688957296E-06</v>
       </c>
       <c r="I8">
-        <v>3.640016717520295e-06</v>
+        <v>3.640016717520295E-06</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -906,13 +906,13 @@
         </is>
       </c>
       <c r="G9">
-        <v>9.082212552045325e-09</v>
+        <v>9.082212552045325E-09</v>
       </c>
       <c r="H9">
-        <v>4.592193721627918e-06</v>
+        <v>4.592193721627918E-06</v>
       </c>
       <c r="I9">
-        <v>3.998563578834692e-06</v>
+        <v>3.998563578834692E-06</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -970,13 +970,13 @@
         </is>
       </c>
       <c r="G10">
-        <v>1.093124506893836e-08</v>
+        <v>1.093124506893836E-08</v>
       </c>
       <c r="H10">
-        <v>4.912987367095073e-06</v>
+        <v>4.912987367095073E-06</v>
       </c>
       <c r="I10">
-        <v>4.277888421130731e-06</v>
+        <v>4.277888421130731E-06</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1034,13 +1034,13 @@
         </is>
       </c>
       <c r="G11">
-        <v>1.674463633685715e-08</v>
+        <v>1.674463633685715E-08</v>
       </c>
       <c r="H11">
-        <v>6.773205398258719e-06</v>
+        <v>6.773205398258719E-06</v>
       </c>
       <c r="I11">
-        <v>5.897637177170951e-06</v>
+        <v>5.897637177170951E-06</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1100,13 +1100,13 @@
         </is>
       </c>
       <c r="G12">
-        <v>2.859418600491823e-08</v>
+        <v>2.859418600491823E-08</v>
       </c>
       <c r="H12">
-        <v>1.051486203544493e-05</v>
+        <v>1.051486203544493E-05</v>
       </c>
       <c r="I12">
-        <v>9.155612093058028e-06</v>
+        <v>9.155612093058028E-06</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1164,13 +1164,13 @@
         </is>
       </c>
       <c r="G13">
-        <v>3.498165864196813e-08</v>
+        <v>3.498165864196813E-08</v>
       </c>
       <c r="H13">
-        <v>1.179173410056342e-05</v>
+        <v>1.179173410056342E-05</v>
       </c>
       <c r="I13">
-        <v>1.02674236680724e-05</v>
+        <v>1.02674236680724E-05</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1228,13 +1228,13 @@
         </is>
       </c>
       <c r="G14">
-        <v>1.20241843075903e-07</v>
+        <v>1.20241843075903E-07</v>
       </c>
       <c r="H14">
-        <v>3.075588103493177e-05</v>
+        <v>3.075588103493177E-05</v>
       </c>
       <c r="I14">
-        <v>2.678008664182726e-05</v>
+        <v>2.678008664182726E-05</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1292,13 +1292,13 @@
         </is>
       </c>
       <c r="G15">
-        <v>1.20241843075903e-07</v>
+        <v>1.20241843075903E-07</v>
       </c>
       <c r="H15">
-        <v>3.075588103493177e-05</v>
+        <v>3.075588103493177E-05</v>
       </c>
       <c r="I15">
-        <v>2.678008664182726e-05</v>
+        <v>2.678008664182726E-05</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1356,13 +1356,13 @@
         </is>
       </c>
       <c r="G16">
-        <v>1.20241843075903e-07</v>
+        <v>1.20241843075903E-07</v>
       </c>
       <c r="H16">
-        <v>3.075588103493177e-05</v>
+        <v>3.075588103493177E-05</v>
       </c>
       <c r="I16">
-        <v>2.678008664182726e-05</v>
+        <v>2.678008664182726E-05</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1420,13 +1420,13 @@
         </is>
       </c>
       <c r="G17">
-        <v>1.216549064422517e-07</v>
+        <v>1.216549064422517E-07</v>
       </c>
       <c r="H17">
-        <v>3.075588103493177e-05</v>
+        <v>3.075588103493177E-05</v>
       </c>
       <c r="I17">
-        <v>2.678008664182726e-05</v>
+        <v>2.678008664182726E-05</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1484,13 +1484,13 @@
         </is>
       </c>
       <c r="G18">
-        <v>1.340473227311227e-07</v>
+        <v>1.340473227311227E-07</v>
       </c>
       <c r="H18">
-        <v>3.189537767337595e-05</v>
+        <v>3.189537767337595E-05</v>
       </c>
       <c r="I18">
-        <v>2.777228122961836e-05</v>
+        <v>2.777228122961836E-05</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1548,13 +1548,13 @@
         </is>
       </c>
       <c r="G19">
-        <v>1.585545640493722e-07</v>
+        <v>1.585545640493722E-07</v>
       </c>
       <c r="H19">
-        <v>3.563073397665059e-05</v>
+        <v>3.563073397665059E-05</v>
       </c>
       <c r="I19">
-        <v>3.102477025199996e-05</v>
+        <v>3.102477025199996E-05</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1613,13 +1613,13 @@
         </is>
       </c>
       <c r="G20">
-        <v>2.31978974638796e-07</v>
+        <v>2.31978974638796E-07</v>
       </c>
       <c r="H20">
-        <v>4.691774762069648e-05</v>
+        <v>4.691774762069648E-05</v>
       </c>
       <c r="I20">
-        <v>4.085271837586375e-05</v>
+        <v>4.085271837586375E-05</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1678,13 +1678,13 @@
         </is>
       </c>
       <c r="G21">
-        <v>2.31978974638796e-07</v>
+        <v>2.31978974638796E-07</v>
       </c>
       <c r="H21">
-        <v>4.691774762069648e-05</v>
+        <v>4.691774762069648E-05</v>
       </c>
       <c r="I21">
-        <v>4.085271837586375e-05</v>
+        <v>4.085271837586375E-05</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1742,13 +1742,13 @@
         </is>
       </c>
       <c r="G22">
-        <v>3.527958890773146e-07</v>
+        <v>3.527958890773146E-07</v>
       </c>
       <c r="H22">
-        <v>6.795520815798751e-05</v>
+        <v>6.795520815798751E-05</v>
       </c>
       <c r="I22">
-        <v>5.91706789399847e-05</v>
+        <v>5.91706789399847E-05</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1806,13 +1806,13 @@
         </is>
       </c>
       <c r="G23">
-        <v>4.537180510774533e-07</v>
+        <v>4.537180510774533E-07</v>
       </c>
       <c r="H23">
-        <v>8.143333660169091e-05</v>
+        <v>8.143333660169091E-05</v>
       </c>
       <c r="I23">
-        <v>7.09064977605251e-05</v>
+        <v>7.09064977605251E-05</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1870,13 +1870,13 @@
         </is>
       </c>
       <c r="G24">
-        <v>4.7777045430621e-07</v>
+        <v>4.7777045430621E-07</v>
       </c>
       <c r="H24">
-        <v>8.143333660169091e-05</v>
+        <v>8.143333660169091E-05</v>
       </c>
       <c r="I24">
-        <v>7.09064977605251e-05</v>
+        <v>7.09064977605251E-05</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1934,13 +1934,13 @@
         </is>
       </c>
       <c r="G25">
-        <v>4.831644198864232e-07</v>
+        <v>4.831644198864232E-07</v>
       </c>
       <c r="H25">
-        <v>8.143333660169091e-05</v>
+        <v>8.143333660169091E-05</v>
       </c>
       <c r="I25">
-        <v>7.09064977605251e-05</v>
+        <v>7.09064977605251E-05</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1998,13 +1998,13 @@
         </is>
       </c>
       <c r="G26">
-        <v>5.789057222469197e-07</v>
+        <v>5.789057222469197E-07</v>
       </c>
       <c r="H26">
-        <v>9.366694585955162e-05</v>
+        <v>9.366694585955162E-05</v>
       </c>
       <c r="I26">
-        <v>8.155867564792393e-05</v>
+        <v>8.155867564792393E-05</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2063,13 +2063,13 @@
         </is>
       </c>
       <c r="G27">
-        <v>6.115291580525984e-07</v>
+        <v>6.115291580525984E-07</v>
       </c>
       <c r="H27">
-        <v>9.421915503551504e-05</v>
+        <v>9.421915503551504E-05</v>
       </c>
       <c r="I27">
-        <v>8.20395010731464e-05</v>
+        <v>8.20395010731464E-05</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2127,13 +2127,13 @@
         </is>
       </c>
       <c r="G28">
-        <v>6.289041250825479e-07</v>
+        <v>6.289041250825479E-07</v>
       </c>
       <c r="H28">
-        <v>9.421915503551504e-05</v>
+        <v>9.421915503551504E-05</v>
       </c>
       <c r="I28">
-        <v>8.20395010731464e-05</v>
+        <v>8.20395010731464E-05</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2192,13 +2192,13 @@
         </is>
       </c>
       <c r="G29">
-        <v>6.678246611265197e-07</v>
+        <v>6.678246611265197E-07</v>
       </c>
       <c r="H29">
-        <v>9.647681265202758e-05</v>
+        <v>9.647681265202758E-05</v>
       </c>
       <c r="I29">
-        <v>8.400531263644116e-05</v>
+        <v>8.400531263644116E-05</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2256,13 +2256,13 @@
         </is>
       </c>
       <c r="G30">
-        <v>7.905976299200639e-07</v>
+        <v>7.905976299200639E-07</v>
       </c>
       <c r="H30">
         <v>0.0001102747383802296</v>
       </c>
       <c r="I30">
-        <v>9.601958873729705e-05</v>
+        <v>9.601958873729705E-05</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2320,7 +2320,7 @@
         </is>
       </c>
       <c r="G31">
-        <v>1.209773895913604e-06</v>
+        <v>1.209773895913604E-06</v>
       </c>
       <c r="H31">
         <v>0.0001631178469656842</v>
@@ -2384,7 +2384,7 @@
         </is>
       </c>
       <c r="G32">
-        <v>1.41831824047908e-06</v>
+        <v>1.41831824047908E-06</v>
       </c>
       <c r="H32">
         <v>0.0001850676542818671</v>
@@ -2449,7 +2449,7 @@
         </is>
       </c>
       <c r="G33">
-        <v>1.568345148764951e-06</v>
+        <v>1.568345148764951E-06</v>
       </c>
       <c r="H33">
         <v>0.0001982486289610695</v>
@@ -2513,7 +2513,7 @@
         </is>
       </c>
       <c r="G34">
-        <v>1.862774436227581e-06</v>
+        <v>1.862774436227581E-06</v>
       </c>
       <c r="H34">
         <v>0.0002268804667388378</v>
@@ -2577,7 +2577,7 @@
         </is>
       </c>
       <c r="G35">
-        <v>1.907029881117549e-06</v>
+        <v>1.907029881117549E-06</v>
       </c>
       <c r="H35">
         <v>0.0002268804667388378</v>
@@ -2641,7 +2641,7 @@
         </is>
       </c>
       <c r="G36">
-        <v>2.07804754227084e-06</v>
+        <v>2.07804754227084E-06</v>
       </c>
       <c r="H36">
         <v>0.0002401629230995871</v>
@@ -2705,7 +2705,7 @@
         </is>
       </c>
       <c r="G37">
-        <v>2.351686113416669e-06</v>
+        <v>2.351686113416669E-06</v>
       </c>
       <c r="H37">
         <v>0.0002642380646880674</v>
@@ -2770,7 +2770,7 @@
         </is>
       </c>
       <c r="G38">
-        <v>2.943298926856706e-06</v>
+        <v>2.943298926856706E-06</v>
       </c>
       <c r="H38">
         <v>0.0003157171464725436</v>
@@ -2834,7 +2834,7 @@
         </is>
       </c>
       <c r="G39">
-        <v>2.965945999000409e-06</v>
+        <v>2.965945999000409E-06</v>
       </c>
       <c r="H39">
         <v>0.0003157171464725436</v>
@@ -2898,7 +2898,7 @@
         </is>
       </c>
       <c r="G40">
-        <v>3.152420439645701e-06</v>
+        <v>3.152420439645701E-06</v>
       </c>
       <c r="H40">
         <v>0.0003269625814965861</v>
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="G41">
-        <v>3.313971018588838e-06</v>
+        <v>3.313971018588838E-06</v>
       </c>
       <c r="H41">
         <v>0.0003297075619687123</v>
@@ -3027,7 +3027,7 @@
         </is>
       </c>
       <c r="G42">
-        <v>3.341906066926379e-06</v>
+        <v>3.341906066926379E-06</v>
       </c>
       <c r="H42">
         <v>0.0003297075619687123</v>
@@ -3091,7 +3091,7 @@
         </is>
       </c>
       <c r="G43">
-        <v>3.702331219030389e-06</v>
+        <v>3.702331219030389E-06</v>
       </c>
       <c r="H43">
         <v>0.0003565697566899505</v>
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="G44">
-        <v>4.118963231710342e-06</v>
+        <v>4.118963231710342E-06</v>
       </c>
       <c r="H44">
         <v>0.0003874699133085659</v>
@@ -3206,7 +3206,7 @@
         </is>
       </c>
       <c r="G45">
-        <v>4.496338542187381e-06</v>
+        <v>4.496338542187381E-06</v>
       </c>
       <c r="H45">
         <v>0.0004133565773442717</v>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="G46">
-        <v>5.107324461801259e-06</v>
+        <v>5.107324461801259E-06</v>
       </c>
       <c r="H46">
         <v>0.0004590917210663576</v>
@@ -3335,7 +3335,7 @@
         </is>
       </c>
       <c r="G47">
-        <v>5.412608968066523e-06</v>
+        <v>5.412608968066523E-06</v>
       </c>
       <c r="H47">
         <v>0.0004759565929528062</v>
@@ -3399,7 +3399,7 @@
         </is>
       </c>
       <c r="G48">
-        <v>5.604931700159812e-06</v>
+        <v>5.604931700159812E-06</v>
       </c>
       <c r="H48">
         <v>0.0004823818878116263</v>
@@ -3463,7 +3463,7 @@
         </is>
       </c>
       <c r="G49">
-        <v>6.072231987245428e-06</v>
+        <v>6.072231987245428E-06</v>
       </c>
       <c r="H49">
         <v>0.0005117120497584948</v>
@@ -3528,7 +3528,7 @@
         </is>
       </c>
       <c r="G50">
-        <v>1.019772601745451e-05</v>
+        <v>1.019772601745451E-05</v>
       </c>
       <c r="H50">
         <v>0.0008418326885837445</v>
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="G51">
-        <v>1.096483918034159e-05</v>
+        <v>1.096483918034159E-05</v>
       </c>
       <c r="H51">
         <v>0.0008684407334688173</v>
@@ -3659,7 +3659,7 @@
         </is>
       </c>
       <c r="G52">
-        <v>1.096483918034159e-05</v>
+        <v>1.096483918034159E-05</v>
       </c>
       <c r="H52">
         <v>0.0008684407334688173</v>
@@ -3723,7 +3723,7 @@
         </is>
       </c>
       <c r="G53">
-        <v>1.116413303841249e-05</v>
+        <v>1.116413303841249E-05</v>
       </c>
       <c r="H53">
         <v>0.0008684407334688173</v>
@@ -3788,7 +3788,7 @@
         </is>
       </c>
       <c r="G54">
-        <v>1.168002695346436e-05</v>
+        <v>1.168002695346436E-05</v>
       </c>
       <c r="H54">
         <v>0.0008914284722030816</v>
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="G55">
-        <v>1.204952464847293e-05</v>
+        <v>1.204952464847293E-05</v>
       </c>
       <c r="H55">
         <v>0.0009025986519087591</v>
@@ -3916,7 +3916,7 @@
         </is>
       </c>
       <c r="G56">
-        <v>1.297337722267735e-05</v>
+        <v>1.297337722267735E-05</v>
       </c>
       <c r="H56">
         <v>0.0009541329248314527</v>
@@ -3980,7 +3980,7 @@
         </is>
       </c>
       <c r="G57">
-        <v>1.340300194595055e-05</v>
+        <v>1.340300194595055E-05</v>
       </c>
       <c r="H57">
         <v>0.0009681275512744638</v>
@@ -4044,7 +4044,7 @@
         </is>
       </c>
       <c r="G58">
-        <v>1.441770023017928e-05</v>
+        <v>1.441770023017928E-05</v>
       </c>
       <c r="H58">
         <v>0.001023150832124126</v>
@@ -4108,7 +4108,7 @@
         </is>
       </c>
       <c r="G59">
-        <v>1.599599878286436e-05</v>
+        <v>1.599599878286436E-05</v>
       </c>
       <c r="H59">
         <v>0.001115583018563557</v>
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="G60">
-        <v>1.669232225371941e-05</v>
+        <v>1.669232225371941E-05</v>
       </c>
       <c r="H60">
         <v>0.001144414296886356</v>
@@ -4236,7 +4236,7 @@
         </is>
       </c>
       <c r="G61">
-        <v>1.739845486616694e-05</v>
+        <v>1.739845486616694E-05</v>
       </c>
       <c r="H61">
         <v>0.001172945832227422</v>
@@ -4300,7 +4300,7 @@
         </is>
       </c>
       <c r="G62">
-        <v>1.772645874871491e-05</v>
+        <v>1.772645874871491E-05</v>
       </c>
       <c r="H62">
         <v>0.001175467633418882</v>
@@ -4364,7 +4364,7 @@
         </is>
       </c>
       <c r="G63">
-        <v>1.83198495512095e-05</v>
+        <v>1.83198495512095E-05</v>
       </c>
       <c r="H63">
         <v>0.001195222442494233</v>
@@ -4428,7 +4428,7 @@
         </is>
       </c>
       <c r="G64">
-        <v>1.86689142033305e-05</v>
+        <v>1.86689142033305E-05</v>
       </c>
       <c r="H64">
         <v>0.00119866282464241</v>
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="G65">
-        <v>1.921581504736971e-05</v>
+        <v>1.921581504736971E-05</v>
       </c>
       <c r="H65">
         <v>0.001214499560415789</v>
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="G66">
-        <v>2.127780479857591e-05</v>
+        <v>2.127780479857591E-05</v>
       </c>
       <c r="H66">
         <v>0.001324134160157531</v>
@@ -4622,7 +4622,7 @@
         </is>
       </c>
       <c r="G67">
-        <v>2.55228215370946e-05</v>
+        <v>2.55228215370946E-05</v>
       </c>
       <c r="H67">
         <v>0.001564239592690116</v>
@@ -4686,7 +4686,7 @@
         </is>
       </c>
       <c r="G68">
-        <v>2.694150938233565e-05</v>
+        <v>2.694150938233565E-05</v>
       </c>
       <c r="H68">
         <v>0.001626543364948473</v>
@@ -4750,7 +4750,7 @@
         </is>
       </c>
       <c r="G69">
-        <v>2.942643197144688e-05</v>
+        <v>2.942643197144688E-05</v>
       </c>
       <c r="H69">
         <v>0.001734069459564027</v>
@@ -4815,7 +4815,7 @@
         </is>
       </c>
       <c r="G70">
-        <v>2.957992403211813e-05</v>
+        <v>2.957992403211813E-05</v>
       </c>
       <c r="H70">
         <v>0.001734069459564027</v>
@@ -4879,7 +4879,7 @@
         </is>
       </c>
       <c r="G71">
-        <v>3.697881901601796e-05</v>
+        <v>3.697881901601796E-05</v>
       </c>
       <c r="H71">
         <v>0.002120518224828006</v>
@@ -4944,7 +4944,7 @@
         </is>
       </c>
       <c r="G72">
-        <v>3.722046822318626e-05</v>
+        <v>3.722046822318626E-05</v>
       </c>
       <c r="H72">
         <v>0.002120518224828006</v>
@@ -5008,7 +5008,7 @@
         </is>
       </c>
       <c r="G73">
-        <v>4.239696276896629e-05</v>
+        <v>4.239696276896629E-05</v>
       </c>
       <c r="H73">
         <v>0.002381884922228731</v>
@@ -5072,7 +5072,7 @@
         </is>
       </c>
       <c r="G74">
-        <v>5.446377092881828e-05</v>
+        <v>5.446377092881828E-05</v>
       </c>
       <c r="H74">
         <v>0.002984729133770767</v>
@@ -5136,7 +5136,7 @@
         </is>
       </c>
       <c r="G75">
-        <v>5.460320294166546e-05</v>
+        <v>5.460320294166546E-05</v>
       </c>
       <c r="H75">
         <v>0.002984729133770767</v>
@@ -5201,7 +5201,7 @@
         </is>
       </c>
       <c r="G76">
-        <v>5.712687529314963e-05</v>
+        <v>5.712687529314963E-05</v>
       </c>
       <c r="H76">
         <v>0.003081042807477203</v>
@@ -5265,7 +5265,7 @@
         </is>
       </c>
       <c r="G77">
-        <v>5.887283191479337e-05</v>
+        <v>5.887283191479337E-05</v>
       </c>
       <c r="H77">
         <v>0.003133429014412358</v>
@@ -5330,7 +5330,7 @@
         </is>
       </c>
       <c r="G78">
-        <v>6.195199523517279e-05</v>
+        <v>6.195199523517279E-05</v>
       </c>
       <c r="H78">
         <v>0.003254491178263298</v>
@@ -5394,7 +5394,7 @@
         </is>
       </c>
       <c r="G79">
-        <v>6.431463723396608e-05</v>
+        <v>6.431463723396608E-05</v>
       </c>
       <c r="H79">
         <v>0.003293072248245479</v>
@@ -5459,7 +5459,7 @@
         </is>
       </c>
       <c r="G80">
-        <v>6.431463723396608e-05</v>
+        <v>6.431463723396608E-05</v>
       </c>
       <c r="H80">
         <v>0.003293072248245479</v>
@@ -5523,7 +5523,7 @@
         </is>
       </c>
       <c r="G81">
-        <v>7.256143566308788e-05</v>
+        <v>7.256143566308788E-05</v>
       </c>
       <c r="H81">
         <v>0.003645180718039407</v>
@@ -5587,7 +5587,7 @@
         </is>
       </c>
       <c r="G82">
-        <v>7.299373007693251e-05</v>
+        <v>7.299373007693251E-05</v>
       </c>
       <c r="H82">
         <v>0.003645180718039407</v>
@@ -5651,7 +5651,7 @@
         </is>
       </c>
       <c r="G83">
-        <v>7.964803427510685e-05</v>
+        <v>7.964803427510685E-05</v>
       </c>
       <c r="H83">
         <v>0.003928979251741551</v>
@@ -5715,7 +5715,7 @@
         </is>
       </c>
       <c r="G84">
-        <v>8.600565557902751e-05</v>
+        <v>8.600565557902751E-05</v>
       </c>
       <c r="H84">
         <v>0.004191480443580317</v>
@@ -5779,7 +5779,7 @@
         </is>
       </c>
       <c r="G85">
-        <v>9.522728096549646e-05</v>
+        <v>9.522728096549646E-05</v>
       </c>
       <c r="H85">
         <v>0.004585647041731348</v>
@@ -15806,13 +15806,13 @@
         </is>
       </c>
       <c r="G241">
-        <v>1.674529971548231e-12</v>
+        <v>1.674529971548231E-12</v>
       </c>
       <c r="H241">
-        <v>6.865572883347746e-10</v>
+        <v>6.865572883347746E-10</v>
       </c>
       <c r="I241">
-        <v>5.975428003735265e-10</v>
+        <v>5.975428003735265E-10</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -15870,13 +15870,13 @@
         </is>
       </c>
       <c r="G242">
-        <v>7.182982122723463e-12</v>
+        <v>7.182982122723463E-12</v>
       </c>
       <c r="H242">
-        <v>9.816742234388733e-10</v>
+        <v>9.816742234388733E-10</v>
       </c>
       <c r="I242">
-        <v>8.543968209134224e-10</v>
+        <v>8.543968209134224E-10</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -15934,13 +15934,13 @@
         </is>
       </c>
       <c r="G243">
-        <v>7.182982122723463e-12</v>
+        <v>7.182982122723463E-12</v>
       </c>
       <c r="H243">
-        <v>9.816742234388733e-10</v>
+        <v>9.816742234388733E-10</v>
       </c>
       <c r="I243">
-        <v>8.543968209134224e-10</v>
+        <v>8.543968209134224E-10</v>
       </c>
       <c r="J243" t="inlineStr">
         <is>
@@ -15998,13 +15998,13 @@
         </is>
       </c>
       <c r="G244">
-        <v>3.510990666554866e-10</v>
+        <v>3.510990666554866E-10</v>
       </c>
       <c r="H244">
-        <v>3.598765433218738e-08</v>
+        <v>3.598765433218738E-08</v>
       </c>
       <c r="I244">
-        <v>3.132173252531841e-08</v>
+        <v>3.132173252531841E-08</v>
       </c>
       <c r="J244" t="inlineStr">
         <is>
@@ -16062,13 +16062,13 @@
         </is>
       </c>
       <c r="G245">
-        <v>6.06459909705533e-08</v>
+        <v>6.06459909705533E-08</v>
       </c>
       <c r="H245">
-        <v>4.972971259585371e-06</v>
+        <v>4.972971259585371E-06</v>
       </c>
       <c r="I245">
-        <v>4.328208618740541e-06</v>
+        <v>4.328208618740541E-06</v>
       </c>
       <c r="J245" t="inlineStr">
         <is>
@@ -16126,13 +16126,13 @@
         </is>
       </c>
       <c r="G246">
-        <v>1.002444745316328e-07</v>
+        <v>1.002444745316328E-07</v>
       </c>
       <c r="H246">
-        <v>6.850039092994907e-06</v>
+        <v>6.850039092994907E-06</v>
       </c>
       <c r="I246">
-        <v>5.961908222144476e-06</v>
+        <v>5.961908222144476E-06</v>
       </c>
       <c r="J246" t="inlineStr">
         <is>
@@ -16190,13 +16190,13 @@
         </is>
       </c>
       <c r="G247">
-        <v>1.607201136617619e-07</v>
+        <v>1.607201136617619E-07</v>
       </c>
       <c r="H247">
-        <v>9.413606657331766e-06</v>
+        <v>9.413606657331766E-06</v>
       </c>
       <c r="I247">
-        <v>8.193100531028161e-06</v>
+        <v>8.193100531028161E-06</v>
       </c>
       <c r="J247" t="inlineStr">
         <is>
@@ -16254,13 +16254,13 @@
         </is>
       </c>
       <c r="G248">
-        <v>9.47277180976961e-07</v>
+        <v>9.47277180976961E-07</v>
       </c>
       <c r="H248">
-        <v>4.854795552506925e-05</v>
+        <v>4.854795552506925E-05</v>
       </c>
       <c r="I248">
-        <v>4.225354794094602e-05</v>
+        <v>4.225354794094602E-05</v>
       </c>
       <c r="J248" t="inlineStr">
         <is>
@@ -16318,7 +16318,7 @@
         </is>
       </c>
       <c r="G249">
-        <v>2.227874950186645e-05</v>
+        <v>2.227874950186645E-05</v>
       </c>
       <c r="H249">
         <v>0.0009346743516622709</v>
@@ -16382,7 +16382,7 @@
         </is>
       </c>
       <c r="G250">
-        <v>2.507662894703654e-05</v>
+        <v>2.507662894703654E-05</v>
       </c>
       <c r="H250">
         <v>0.0009346743516622709</v>
@@ -16446,7 +16446,7 @@
         </is>
       </c>
       <c r="G251">
-        <v>2.507662894703654e-05</v>
+        <v>2.507662894703654E-05</v>
       </c>
       <c r="H251">
         <v>0.0009346743516622709</v>
@@ -16510,7 +16510,7 @@
         </is>
       </c>
       <c r="G252">
-        <v>3.11400874515041e-05</v>
+        <v>3.11400874515041E-05</v>
       </c>
       <c r="H252">
         <v>0.00106395298792639</v>
@@ -16574,7 +16574,7 @@
         </is>
       </c>
       <c r="G253">
-        <v>6.409712882446523e-05</v>
+        <v>6.409712882446523E-05</v>
       </c>
       <c r="H253">
         <v>0.001890069509514902</v>
@@ -16638,7 +16638,7 @@
         </is>
       </c>
       <c r="G254">
-        <v>6.453895886148446e-05</v>
+        <v>6.453895886148446E-05</v>
       </c>
       <c r="H254">
         <v>0.001890069509514902</v>
@@ -16702,7 +16702,7 @@
         </is>
       </c>
       <c r="G255">
-        <v>8.232796302219709e-05</v>
+        <v>8.232796302219709E-05</v>
       </c>
       <c r="H255">
         <v>0.002250297655940054</v>
@@ -17534,13 +17534,13 @@
         </is>
       </c>
       <c r="G268">
-        <v>3.634708081848018e-14</v>
+        <v>3.634708081848018E-14</v>
       </c>
       <c r="H268">
-        <v>2.046340650080434e-11</v>
+        <v>2.046340650080434E-11</v>
       </c>
       <c r="I268">
-        <v>1.836484083460051e-11</v>
+        <v>1.836484083460051E-11</v>
       </c>
       <c r="J268" t="inlineStr">
         <is>
@@ -17598,13 +17598,13 @@
         </is>
       </c>
       <c r="G269">
-        <v>7.422748718822332e-14</v>
+        <v>7.422748718822332E-14</v>
       </c>
       <c r="H269">
-        <v>2.089503764348486e-11</v>
+        <v>2.089503764348486E-11</v>
       </c>
       <c r="I269">
-        <v>1.875220728965642e-11</v>
+        <v>1.875220728965642E-11</v>
       </c>
       <c r="J269" t="inlineStr">
         <is>
@@ -17662,13 +17662,13 @@
         </is>
       </c>
       <c r="G270">
-        <v>1.752641895026858e-13</v>
+        <v>1.752641895026858E-13</v>
       </c>
       <c r="H270">
-        <v>3.289124623000404e-11</v>
+        <v>3.289124623000404E-11</v>
       </c>
       <c r="I270">
-        <v>2.951817928466288e-11</v>
+        <v>2.951817928466288E-11</v>
       </c>
       <c r="J270" t="inlineStr">
         <is>
@@ -17726,13 +17726,13 @@
         </is>
       </c>
       <c r="G271">
-        <v>4.768579637916504e-10</v>
+        <v>4.768579637916504E-10</v>
       </c>
       <c r="H271">
-        <v>6.711775840367479e-08</v>
+        <v>6.711775840367479E-08</v>
       </c>
       <c r="I271">
-        <v>6.023469016315584e-08</v>
+        <v>6.023469016315584E-08</v>
       </c>
       <c r="J271" t="inlineStr">
         <is>
@@ -17790,13 +17790,13 @@
         </is>
       </c>
       <c r="G272">
-        <v>1.54604928625759e-08</v>
+        <v>1.54604928625759E-08</v>
       </c>
       <c r="H272">
-        <v>1.740851496326046e-06</v>
+        <v>1.740851496326046E-06</v>
       </c>
       <c r="I272">
-        <v>1.562323489270828e-06</v>
+        <v>1.562323489270828E-06</v>
       </c>
       <c r="J272" t="inlineStr">
         <is>
@@ -17854,13 +17854,13 @@
         </is>
       </c>
       <c r="G273">
-        <v>8.713868191863613e-08</v>
+        <v>8.713868191863613E-08</v>
       </c>
       <c r="H273">
-        <v>8.17651298669869e-06</v>
+        <v>8.17651298669869E-06</v>
       </c>
       <c r="I273">
-        <v>7.337994266832517e-06</v>
+        <v>7.337994266832517E-06</v>
       </c>
       <c r="J273" t="inlineStr">
         <is>
@@ -17918,7 +17918,7 @@
         </is>
       </c>
       <c r="G274">
-        <v>2.077964328456312e-06</v>
+        <v>2.077964328456312E-06</v>
       </c>
       <c r="H274">
         <v>0.000167127702417272</v>
@@ -17982,7 +17982,7 @@
         </is>
       </c>
       <c r="G275">
-        <v>3.643781582138549e-06</v>
+        <v>3.643781582138549E-06</v>
       </c>
       <c r="H275">
         <v>0.0002564311288430004</v>
@@ -18046,7 +18046,7 @@
         </is>
       </c>
       <c r="G276">
-        <v>9.147604551364934e-06</v>
+        <v>9.147604551364934E-06</v>
       </c>
       <c r="H276">
         <v>0.000572233484713162</v>
@@ -18110,7 +18110,7 @@
         </is>
       </c>
       <c r="G277">
-        <v>1.270155841205904e-05</v>
+        <v>1.270155841205904E-05</v>
       </c>
       <c r="H277">
         <v>0.000715097738598924</v>
@@ -18174,7 +18174,7 @@
         </is>
       </c>
       <c r="G278">
-        <v>1.961561677873156e-05</v>
+        <v>1.961561677873156E-05</v>
       </c>
       <c r="H278">
         <v>0.001003962931493261</v>
@@ -18238,7 +18238,7 @@
         </is>
       </c>
       <c r="G279">
-        <v>4.180576175236572e-05</v>
+        <v>4.180576175236572E-05</v>
       </c>
       <c r="H279">
         <v>0.001919773089061648</v>
@@ -18302,7 +18302,7 @@
         </is>
       </c>
       <c r="G280">
-        <v>4.432868589307536e-05</v>
+        <v>4.432868589307536E-05</v>
       </c>
       <c r="H280">
         <v>0.001919773089061648</v>
@@ -19039,13 +19039,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>1.703096750930508e-09</v>
+        <v>1.703096750930508E-09</v>
       </c>
       <c r="H2">
-        <v>8.013070213128041e-06</v>
+        <v>8.013070213128041E-06</v>
       </c>
       <c r="I2">
-        <v>7.430880034323111e-06</v>
+        <v>7.430880034323111E-06</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -19103,13 +19103,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>4.909421475125471e-09</v>
+        <v>4.909421475125471E-09</v>
       </c>
       <c r="H3">
-        <v>1.154941402023267e-05</v>
+        <v>1.154941402023267E-05</v>
       </c>
       <c r="I3">
-        <v>1.071029053389215e-05</v>
+        <v>1.071029053389215E-05</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -19167,7 +19167,7 @@
         </is>
       </c>
       <c r="G4">
-        <v>9.728561293658429e-08</v>
+        <v>9.728561293658429E-08</v>
       </c>
       <c r="H4">
         <v>0.0001525762696222097</v>
@@ -19231,7 +19231,7 @@
         </is>
       </c>
       <c r="G5">
-        <v>3.403564133997522e-07</v>
+        <v>3.403564133997522E-07</v>
       </c>
       <c r="H5">
         <v>0.0004003442312614586</v>
@@ -19295,7 +19295,7 @@
         </is>
       </c>
       <c r="G6">
-        <v>5.74585354078421e-07</v>
+        <v>5.74585354078421E-07</v>
       </c>
       <c r="H6">
         <v>0.0005406848181877941</v>
@@ -19359,7 +19359,7 @@
         </is>
       </c>
       <c r="G7">
-        <v>1.687687757084273e-06</v>
+        <v>1.687687757084273E-06</v>
       </c>
       <c r="H7">
         <v>0.001323428482846917</v>
@@ -19423,7 +19423,7 @@
         </is>
       </c>
       <c r="G8">
-        <v>1.974224515162653e-06</v>
+        <v>1.974224515162653E-06</v>
       </c>
       <c r="H8">
         <v>0.001326960906262898</v>
@@ -19487,7 +19487,7 @@
         </is>
       </c>
       <c r="G9">
-        <v>2.498790278906904e-06</v>
+        <v>2.498790278906904E-06</v>
       </c>
       <c r="H9">
         <v>0.001469601032782123</v>
@@ -19551,7 +19551,7 @@
         </is>
       </c>
       <c r="G10">
-        <v>4.492474474434408e-06</v>
+        <v>4.492474474434408E-06</v>
       </c>
       <c r="H10">
         <v>0.00234856582246821</v>
@@ -19615,7 +19615,7 @@
         </is>
       </c>
       <c r="G11">
-        <v>6.779908664909922e-06</v>
+        <v>6.779908664909922E-06</v>
       </c>
       <c r="H11">
         <v>0.002699229217002326</v>
@@ -19679,7 +19679,7 @@
         </is>
       </c>
       <c r="G12">
-        <v>7.182786002137921e-06</v>
+        <v>7.182786002137921E-06</v>
       </c>
       <c r="H12">
         <v>0.002699229217002326</v>
@@ -19743,7 +19743,7 @@
         </is>
       </c>
       <c r="G13">
-        <v>7.22482717931057e-06</v>
+        <v>7.22482717931057E-06</v>
       </c>
       <c r="H13">
         <v>0.002699229217002326</v>
@@ -19807,7 +19807,7 @@
         </is>
       </c>
       <c r="G14">
-        <v>7.458019090548403e-06</v>
+        <v>7.458019090548403E-06</v>
       </c>
       <c r="H14">
         <v>0.002699229217002326</v>
@@ -19871,7 +19871,7 @@
         </is>
       </c>
       <c r="G15">
-        <v>1.049991166153878e-05</v>
+        <v>1.049991166153878E-05</v>
       </c>
       <c r="H15">
         <v>0.003528720311967139</v>
@@ -19935,7 +19935,7 @@
         </is>
       </c>
       <c r="G16">
-        <v>1.94222109535252e-05</v>
+        <v>1.94222109535252E-05</v>
       </c>
       <c r="H16">
         <v>0.006092100169089073</v>
@@ -19999,7 +19999,7 @@
         </is>
       </c>
       <c r="G17">
-        <v>2.714811610236439e-05</v>
+        <v>2.714811610236439E-05</v>
       </c>
       <c r="H17">
         <v>0.007983242891351531</v>
@@ -20064,7 +20064,7 @@
         </is>
       </c>
       <c r="G18">
-        <v>3.850715404940927e-05</v>
+        <v>3.850715404940927E-05</v>
       </c>
       <c r="H18">
         <v>0.01006534221124837</v>
@@ -20128,7 +20128,7 @@
         </is>
       </c>
       <c r="G19">
-        <v>3.850715404940927e-05</v>
+        <v>3.850715404940927E-05</v>
       </c>
       <c r="H19">
         <v>0.01006534221124837</v>
@@ -20192,7 +20192,7 @@
         </is>
       </c>
       <c r="G20">
-        <v>4.094677195568746e-05</v>
+        <v>4.094677195568746E-05</v>
       </c>
       <c r="H20">
         <v>0.01013971379218471</v>
@@ -20256,7 +20256,7 @@
         </is>
       </c>
       <c r="G21">
-        <v>5.616952220659327e-05</v>
+        <v>5.616952220659327E-05</v>
       </c>
       <c r="H21">
         <v>0.01321388009910106</v>
@@ -20320,7 +20320,7 @@
         </is>
       </c>
       <c r="G22">
-        <v>6.142240143840832e-05</v>
+        <v>6.142240143840832E-05</v>
       </c>
       <c r="H22">
         <v>0.01358913284643349</v>
@@ -20384,7 +20384,7 @@
         </is>
       </c>
       <c r="G23">
-        <v>6.806754652927528e-05</v>
+        <v>6.806754652927528E-05</v>
       </c>
       <c r="H23">
         <v>0.01358913284643349</v>
@@ -20448,7 +20448,7 @@
         </is>
       </c>
       <c r="G24">
-        <v>6.931757456204116e-05</v>
+        <v>6.931757456204116E-05</v>
       </c>
       <c r="H24">
         <v>0.01358913284643349</v>
@@ -20512,7 +20512,7 @@
         </is>
       </c>
       <c r="G25">
-        <v>6.931757456204116e-05</v>
+        <v>6.931757456204116E-05</v>
       </c>
       <c r="H25">
         <v>0.01358913284643349</v>
@@ -20576,7 +20576,7 @@
         </is>
       </c>
       <c r="G26">
-        <v>7.225545452013631e-05</v>
+        <v>7.225545452013631E-05</v>
       </c>
       <c r="H26">
         <v>0.01359847654068965</v>
@@ -20640,7 +20640,7 @@
         </is>
       </c>
       <c r="G27">
-        <v>7.654658655255029e-05</v>
+        <v>7.654658655255029E-05</v>
       </c>
       <c r="H27">
         <v>0.01385198806652881</v>
@@ -20704,7 +20704,7 @@
         </is>
       </c>
       <c r="G28">
-        <v>9.860060428443174e-05</v>
+        <v>9.860060428443174E-05</v>
       </c>
       <c r="H28">
         <v>0.01718206826512042</v>
@@ -23401,13 +23401,13 @@
         </is>
       </c>
       <c r="G70">
-        <v>1.078652830004532e-12</v>
+        <v>1.078652830004532E-12</v>
       </c>
       <c r="H70">
-        <v>5.091241357621393e-10</v>
+        <v>5.091241357621393E-10</v>
       </c>
       <c r="I70">
-        <v>4.746072452019942e-10</v>
+        <v>4.746072452019942E-10</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -23465,13 +23465,13 @@
         </is>
       </c>
       <c r="G71">
-        <v>1.010887781768046e-10</v>
+        <v>1.010887781768046E-10</v>
       </c>
       <c r="H71">
-        <v>2.385695164972589e-08</v>
+        <v>2.385695164972589E-08</v>
       </c>
       <c r="I71">
-        <v>2.223953119889702e-08</v>
+        <v>2.223953119889702E-08</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -23529,13 +23529,13 @@
         </is>
       </c>
       <c r="G72">
-        <v>5.988292148385169e-07</v>
+        <v>5.988292148385169E-07</v>
       </c>
       <c r="H72">
-        <v>9.421579646792666e-05</v>
+        <v>9.421579646792666E-05</v>
       </c>
       <c r="I72">
-        <v>8.782828484298247e-05</v>
+        <v>8.782828484298247E-05</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -23593,7 +23593,7 @@
         </is>
       </c>
       <c r="G73">
-        <v>1.356819856741865e-06</v>
+        <v>1.356819856741865E-06</v>
       </c>
       <c r="H73">
         <v>0.0001575802805965911</v>
@@ -23657,7 +23657,7 @@
         </is>
       </c>
       <c r="G74">
-        <v>1.855278616562779e-06</v>
+        <v>1.855278616562779E-06</v>
       </c>
       <c r="H74">
         <v>0.0001575802805965911</v>
@@ -23721,7 +23721,7 @@
         </is>
       </c>
       <c r="G75">
-        <v>2.874178102942802e-06</v>
+        <v>2.874178102942802E-06</v>
       </c>
       <c r="H75">
         <v>0.0001575802805965911</v>
@@ -23785,7 +23785,7 @@
         </is>
       </c>
       <c r="G76">
-        <v>2.934770763935013e-06</v>
+        <v>2.934770763935013E-06</v>
       </c>
       <c r="H76">
         <v>0.0001575802805965911</v>
@@ -23849,7 +23849,7 @@
         </is>
       </c>
       <c r="G77">
-        <v>3.141315844879002e-06</v>
+        <v>3.141315844879002E-06</v>
       </c>
       <c r="H77">
         <v>0.0001575802805965911</v>
@@ -23913,7 +23913,7 @@
         </is>
       </c>
       <c r="G78">
-        <v>3.377127770443845e-06</v>
+        <v>3.377127770443845E-06</v>
       </c>
       <c r="H78">
         <v>0.0001575802805965911</v>
@@ -23977,7 +23977,7 @@
         </is>
       </c>
       <c r="G79">
-        <v>3.611098433439241e-06</v>
+        <v>3.611098433439241E-06</v>
       </c>
       <c r="H79">
         <v>0.0001575802805965911</v>
@@ -24041,7 +24041,7 @@
         </is>
       </c>
       <c r="G80">
-        <v>3.672421793564623e-06</v>
+        <v>3.672421793564623E-06</v>
       </c>
       <c r="H80">
         <v>0.0001575802805965911</v>
@@ -24105,7 +24105,7 @@
         </is>
       </c>
       <c r="G81">
-        <v>2.421395820665763e-05</v>
+        <v>2.421395820665763E-05</v>
       </c>
       <c r="H81">
         <v>0.000879152944118646</v>
@@ -24169,7 +24169,7 @@
         </is>
       </c>
       <c r="G82">
-        <v>2.421395820665763e-05</v>
+        <v>2.421395820665763E-05</v>
       </c>
       <c r="H82">
         <v>0.000879152944118646</v>
@@ -24233,7 +24233,7 @@
         </is>
       </c>
       <c r="G83">
-        <v>3.894119199000347e-05</v>
+        <v>3.894119199000347E-05</v>
       </c>
       <c r="H83">
         <v>0.001312874472805831</v>
@@ -24297,13 +24297,13 @@
         </is>
       </c>
       <c r="G84">
-        <v>4.596321321299576e-09</v>
+        <v>4.596321321299576E-09</v>
       </c>
       <c r="H84">
-        <v>3.364507207191289e-06</v>
+        <v>3.364507207191289E-06</v>
       </c>
       <c r="I84">
-        <v>3.072277935816032e-06</v>
+        <v>3.072277935816032E-06</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -24361,13 +24361,13 @@
         </is>
       </c>
       <c r="G85">
-        <v>2.309561756590962e-08</v>
+        <v>2.309561756590962E-08</v>
       </c>
       <c r="H85">
-        <v>8.45299602912292e-06</v>
+        <v>8.45299602912292E-06</v>
       </c>
       <c r="I85">
-        <v>7.718798502290845e-06</v>
+        <v>7.718798502290845E-06</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -24425,13 +24425,13 @@
         </is>
       </c>
       <c r="G86">
-        <v>5.651542176188484e-08</v>
+        <v>5.651542176188484E-08</v>
       </c>
       <c r="H86">
-        <v>1.37897629098999e-05</v>
+        <v>1.37897629098999E-05</v>
       </c>
       <c r="I86">
-        <v>1.25920325679989e-05</v>
+        <v>1.25920325679989E-05</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -24489,7 +24489,7 @@
         </is>
       </c>
       <c r="G87">
-        <v>1.338721696768284e-06</v>
+        <v>1.338721696768284E-06</v>
       </c>
       <c r="H87">
         <v>0.0002449860705085961</v>
@@ -24553,7 +24553,7 @@
         </is>
       </c>
       <c r="G88">
-        <v>1.288308353623211e-05</v>
+        <v>1.288308353623211E-05</v>
       </c>
       <c r="H88">
         <v>0.001886083429704382</v>
@@ -24617,7 +24617,7 @@
         </is>
       </c>
       <c r="G89">
-        <v>2.104262638243663e-05</v>
+        <v>2.104262638243663E-05</v>
       </c>
       <c r="H89">
         <v>0.002567200418657269</v>
@@ -24681,7 +24681,7 @@
         </is>
       </c>
       <c r="G90">
-        <v>2.668919018180057e-05</v>
+        <v>2.668919018180057E-05</v>
       </c>
       <c r="H90">
         <v>0.002790926744725431</v>
@@ -24745,7 +24745,7 @@
         </is>
       </c>
       <c r="G91">
-        <v>4.962985537111503e-05</v>
+        <v>4.962985537111503E-05</v>
       </c>
       <c r="H91">
         <v>0.004541131766457025</v>
@@ -24809,7 +24809,7 @@
         </is>
       </c>
       <c r="G92">
-        <v>8.421356709962425e-05</v>
+        <v>8.421356709962425E-05</v>
       </c>
       <c r="H92">
         <v>0.006849370124102772</v>
@@ -25612,13 +25612,13 @@
         </is>
       </c>
       <c r="G2">
-        <v>7.863051032199365e-10</v>
+        <v>7.863051032199365E-10</v>
       </c>
       <c r="H2">
-        <v>1.479039899156701e-06</v>
+        <v>1.479039899156701E-06</v>
       </c>
       <c r="I2">
-        <v>1.418659944125233e-06</v>
+        <v>1.418659944125233E-06</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -25662,13 +25662,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>1.755976174049004e-08</v>
+        <v>1.755976174049004E-08</v>
       </c>
       <c r="H3">
-        <v>1.488022248282995e-05</v>
+        <v>1.488022248282995E-05</v>
       </c>
       <c r="I3">
-        <v>1.427275600076697e-05</v>
+        <v>1.427275600076697E-05</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -25726,13 +25726,13 @@
         </is>
       </c>
       <c r="G4">
-        <v>2.373241225331731e-08</v>
+        <v>2.373241225331731E-08</v>
       </c>
       <c r="H4">
-        <v>1.488022248282995e-05</v>
+        <v>1.488022248282995E-05</v>
       </c>
       <c r="I4">
-        <v>1.427275600076697e-05</v>
+        <v>1.427275600076697E-05</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -25790,13 +25790,13 @@
         </is>
       </c>
       <c r="G5">
-        <v>9.849234609613975e-08</v>
+        <v>9.849234609613975E-08</v>
       </c>
       <c r="H5">
-        <v>4.631602575170972e-05</v>
+        <v>4.631602575170972E-05</v>
       </c>
       <c r="I5">
-        <v>4.442523189704831e-05</v>
+        <v>4.442523189704831E-05</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -25854,7 +25854,7 @@
         </is>
       </c>
       <c r="G6">
-        <v>7.849539074814427e-07</v>
+        <v>7.849539074814427E-07</v>
       </c>
       <c r="H6">
         <v>0.0002952996599945187</v>
@@ -25919,7 +25919,7 @@
         </is>
       </c>
       <c r="G7">
-        <v>2.069856917715545e-06</v>
+        <v>2.069856917715545E-06</v>
       </c>
       <c r="H7">
         <v>0.0006489001437038233</v>
@@ -25983,7 +25983,7 @@
         </is>
       </c>
       <c r="G8">
-        <v>2.446723461493277e-06</v>
+        <v>2.446723461493277E-06</v>
       </c>
       <c r="H8">
         <v>0.0006574695472955507</v>
@@ -26047,7 +26047,7 @@
         </is>
       </c>
       <c r="G9">
-        <v>5.01592539367213e-06</v>
+        <v>5.01592539367213E-06</v>
       </c>
       <c r="H9">
         <v>0.001170322550628897</v>
@@ -26112,7 +26112,7 @@
         </is>
       </c>
       <c r="G10">
-        <v>5.5996294288464e-06</v>
+        <v>5.5996294288464E-06</v>
       </c>
       <c r="H10">
         <v>0.001170322550628897</v>
@@ -26177,7 +26177,7 @@
         </is>
       </c>
       <c r="G11">
-        <v>7.418732167825847e-06</v>
+        <v>7.418732167825847E-06</v>
       </c>
       <c r="H11">
         <v>0.001262468062208104</v>
@@ -26242,7 +26242,7 @@
         </is>
       </c>
       <c r="G12">
-        <v>7.418732167825847e-06</v>
+        <v>7.418732167825847E-06</v>
       </c>
       <c r="H12">
         <v>0.001262468062208104</v>
@@ -26306,7 +26306,7 @@
         </is>
       </c>
       <c r="G13">
-        <v>8.054022725410551e-06</v>
+        <v>8.054022725410551E-06</v>
       </c>
       <c r="H13">
         <v>0.001262468062208104</v>
@@ -26370,7 +26370,7 @@
         </is>
       </c>
       <c r="G14">
-        <v>9.63047450314467e-06</v>
+        <v>9.63047450314467E-06</v>
       </c>
       <c r="H14">
         <v>0.001393455580031932</v>
@@ -26435,7 +26435,7 @@
         </is>
       </c>
       <c r="G15">
-        <v>1.231529510989792e-05</v>
+        <v>1.231529510989792E-05</v>
       </c>
       <c r="H15">
         <v>0.001606446949299756</v>
@@ -26499,7 +26499,7 @@
         </is>
       </c>
       <c r="G16">
-        <v>1.281058173285292e-05</v>
+        <v>1.281058173285292E-05</v>
       </c>
       <c r="H16">
         <v>0.001606446949299756</v>
@@ -26563,7 +26563,7 @@
         </is>
       </c>
       <c r="G17">
-        <v>1.648415872167726e-05</v>
+        <v>1.648415872167726E-05</v>
       </c>
       <c r="H17">
         <v>0.001937918909717183</v>
@@ -26627,7 +26627,7 @@
         </is>
       </c>
       <c r="G18">
-        <v>2.019241310680123e-05</v>
+        <v>2.019241310680123E-05</v>
       </c>
       <c r="H18">
         <v>0.002234231120817242</v>
@@ -26692,7 +26692,7 @@
         </is>
       </c>
       <c r="G19">
-        <v>2.869954215419188e-05</v>
+        <v>2.869954215419188E-05</v>
       </c>
       <c r="H19">
         <v>0.002999102155113052</v>
@@ -26756,7 +26756,7 @@
         </is>
       </c>
       <c r="G20">
-        <v>3.778821584137843e-05</v>
+        <v>3.778821584137843E-05</v>
       </c>
       <c r="H20">
         <v>0.003741033368296465</v>
@@ -26821,7 +26821,7 @@
         </is>
       </c>
       <c r="G21">
-        <v>4.521087036398687e-05</v>
+        <v>4.521087036398687E-05</v>
       </c>
       <c r="H21">
         <v>0.004252082357732966</v>
@@ -26886,7 +26886,7 @@
         </is>
       </c>
       <c r="G22">
-        <v>5.718057886044971e-05</v>
+        <v>5.718057886044971E-05</v>
       </c>
       <c r="H22">
         <v>0.00512174613507171</v>
@@ -26952,7 +26952,7 @@
         </is>
       </c>
       <c r="G23">
-        <v>6.300609038431924e-05</v>
+        <v>6.300609038431924E-05</v>
       </c>
       <c r="H23">
         <v>0.005387020727859295</v>
@@ -27016,7 +27016,7 @@
         </is>
       </c>
       <c r="G24">
-        <v>7.732291219089681e-05</v>
+        <v>7.732291219089681E-05</v>
       </c>
       <c r="H24">
         <v>0.006323669470916387</v>
@@ -27081,7 +27081,7 @@
         </is>
       </c>
       <c r="G25">
-        <v>8.611259824223837e-05</v>
+        <v>8.611259824223837E-05</v>
       </c>
       <c r="H25">
         <v>0.006347138461719262</v>
@@ -27147,7 +27147,7 @@
         </is>
       </c>
       <c r="G26">
-        <v>8.611259824223837e-05</v>
+        <v>8.611259824223837E-05</v>
       </c>
       <c r="H26">
         <v>0.006347138461719262</v>
@@ -27211,7 +27211,7 @@
         </is>
       </c>
       <c r="G27">
-        <v>8.773290803014399e-05</v>
+        <v>8.773290803014399E-05</v>
       </c>
       <c r="H27">
         <v>0.006347138461719262</v>
@@ -28111,13 +28111,13 @@
         </is>
       </c>
       <c r="G41">
-        <v>1.704896542032116e-10</v>
+        <v>1.704896542032116E-10</v>
       </c>
       <c r="H41">
-        <v>3.460939980325197e-08</v>
+        <v>3.460939980325197E-08</v>
       </c>
       <c r="I41">
-        <v>2.889350981759692e-08</v>
+        <v>2.889350981759692E-08</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -28175,13 +28175,13 @@
         </is>
       </c>
       <c r="G42">
-        <v>2.757437492556785e-07</v>
+        <v>2.757437492556785E-07</v>
       </c>
       <c r="H42">
-        <v>2.798799054945137e-05</v>
+        <v>2.798799054945137E-05</v>
       </c>
       <c r="I42">
-        <v>2.336565454219171e-05</v>
+        <v>2.336565454219171E-05</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -28239,7 +28239,7 @@
         </is>
       </c>
       <c r="G43">
-        <v>4.415612531833085e-06</v>
+        <v>4.415612531833085E-06</v>
       </c>
       <c r="H43">
         <v>0.0002987897813207054</v>
@@ -28303,7 +28303,7 @@
         </is>
       </c>
       <c r="G44">
-        <v>6.973622132036663e-06</v>
+        <v>6.973622132036663E-06</v>
       </c>
       <c r="H44">
         <v>0.0003539113232008607</v>
@@ -28367,7 +28367,7 @@
         </is>
       </c>
       <c r="G45">
-        <v>5.273187208628111e-05</v>
+        <v>5.273187208628111E-05</v>
       </c>
       <c r="H45">
         <v>0.002140914006703013</v>
@@ -29455,7 +29455,7 @@
         </is>
       </c>
       <c r="G62">
-        <v>8.466038227444295e-06</v>
+        <v>8.466038227444295E-06</v>
       </c>
       <c r="H62">
         <v>0.002378956741911847</v>
@@ -29519,7 +29519,7 @@
         </is>
       </c>
       <c r="G63">
-        <v>2.039355465557459e-05</v>
+        <v>2.039355465557459E-05</v>
       </c>
       <c r="H63">
         <v>0.002441982784823836</v>
@@ -29583,7 +29583,7 @@
         </is>
       </c>
       <c r="G64">
-        <v>2.607099058530785e-05</v>
+        <v>2.607099058530785E-05</v>
       </c>
       <c r="H64">
         <v>0.002441982784823836</v>
@@ -29648,7 +29648,7 @@
         </is>
       </c>
       <c r="G65">
-        <v>5.875383169606365e-05</v>
+        <v>5.875383169606365E-05</v>
       </c>
       <c r="H65">
         <v>0.004127456676648471</v>
@@ -29712,7 +29712,7 @@
         </is>
       </c>
       <c r="G66">
-        <v>8.135843824683454e-05</v>
+        <v>8.135843824683454E-05</v>
       </c>
       <c r="H66">
         <v>0.004572344229472101</v>

</xml_diff>